<commit_message>
added basal maturation rate
</commit_message>
<xml_diff>
--- a/Two_Pool_and_Maturation/rate_matrix_Maturation_sensor.xlsx
+++ b/Two_Pool_and_Maturation/rate_matrix_Maturation_sensor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espru\OneDrive\Documents\GitHub\SynapseModel\Two_Pool_and_Maturation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92DD781-8692-4512-80C1-3C8DBDA60554}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69D6DD7-47F1-4093-8F31-8490F9477BC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
@@ -17,17 +17,18 @@
     <sheet name="ParallelMaturationAndPriming" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="b">ParallelMaturationAndPriming!$B$55</definedName>
-    <definedName name="f">ParallelMaturationAndPriming!$B$56</definedName>
-    <definedName name="k_mature">ParallelMaturationAndPriming!$B$49</definedName>
-    <definedName name="k_off">ParallelMaturationAndPriming!$B$54</definedName>
-    <definedName name="k_on">ParallelMaturationAndPriming!$B$53</definedName>
-    <definedName name="k_prime">ParallelMaturationAndPriming!$B$51</definedName>
+    <definedName name="b">ParallelMaturationAndPriming!$B$56</definedName>
+    <definedName name="f">ParallelMaturationAndPriming!$B$57</definedName>
+    <definedName name="k_mature">ParallelMaturationAndPriming!$B$50</definedName>
+    <definedName name="k_mature_basal">ParallelMaturationAndPriming!$B$49</definedName>
+    <definedName name="k_off">ParallelMaturationAndPriming!$B$55</definedName>
+    <definedName name="k_on">ParallelMaturationAndPriming!$B$54</definedName>
+    <definedName name="k_prime">ParallelMaturationAndPriming!$B$52</definedName>
     <definedName name="k_refill">ParallelMaturationAndPriming!$B$48</definedName>
-    <definedName name="k_unmature">ParallelMaturationAndPriming!$B$50</definedName>
-    <definedName name="k_unprime">ParallelMaturationAndPriming!$B$52</definedName>
-    <definedName name="M_plus">ParallelMaturationAndPriming!$B$57</definedName>
-    <definedName name="P_plus">ParallelMaturationAndPriming!$B$58</definedName>
+    <definedName name="k_unmature">ParallelMaturationAndPriming!$B$51</definedName>
+    <definedName name="k_unprime">ParallelMaturationAndPriming!$B$53</definedName>
+    <definedName name="M_plus">ParallelMaturationAndPriming!$B$58</definedName>
+    <definedName name="P_plus">ParallelMaturationAndPriming!$B$59</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="true" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +38,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="85">
   <si>
     <t>Prime(0,0)</t>
   </si>
@@ -276,9 +279,6 @@
     <t>k_refill</t>
   </si>
   <si>
-    <t>Ca Dependence (binary)</t>
-  </si>
-  <si>
     <t>k_mature</t>
   </si>
   <si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>k_mature_basal</t>
+  </si>
+  <si>
+    <t>Ca Dependence</t>
   </si>
 </sst>
 </file>
@@ -328,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,7 +373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.24997711111789"/>
+        <fgColor theme="2" tint="-0.24994659260842"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,8 +383,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.24994659260842"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="305">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -394,307 +406,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="319">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
@@ -730,6 +446,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" wrapText="true"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
@@ -738,302 +460,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="115" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="116" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="117" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="120" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="121" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="238" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="239" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="240" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="241" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="242" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="243" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="244" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="245" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="246" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2338,10 +1764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB47B66-8A4C-49E3-901F-F956FCB68ADB}">
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="true" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,80 +1856,80 @@
       <c r="C2" s="11">
         <v>0</v>
       </c>
-      <c r="D2" s="14" t="str">
+      <c r="D2" s="14">
         <f>M_plus</f>
-        <v>M_plus</v>
-      </c>
-      <c r="E2" s="14" t="str">
+        <v>3.5E-4</v>
+      </c>
+      <c r="E2" s="14">
         <f>P_plus</f>
-        <v>P_plus</v>
+        <v>0</v>
       </c>
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="14" t="e">
+      <c r="G2" s="14">
         <f>M_plus + P_plus</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H2" s="14" t="e">
+        <v>3.5E-4</v>
+      </c>
+      <c r="H2" s="14">
         <f>M_plus*f</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I2" s="14" t="e">
+        <v>1.2249999999999999E-7</v>
+      </c>
+      <c r="I2" s="14">
         <f>M_plus*f^2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J2" s="14" t="e">
+        <v>4.2874999999999994E-11</v>
+      </c>
+      <c r="J2" s="14">
         <f>M_plus*f^3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K2" s="14" t="e">
+        <v>1.5006249999999997E-14</v>
+      </c>
+      <c r="K2" s="14">
         <f>M_plus*f^4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L2" s="14" t="e">
+        <v>5.2521874999999988E-18</v>
+      </c>
+      <c r="L2" s="14">
         <f>M_plus*f^5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M2" s="14" t="e">
+        <v>1.8382656249999994E-21</v>
+      </c>
+      <c r="M2" s="14">
         <f>P_plus*f</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N2" s="14" t="e">
+        <v>0</v>
+      </c>
+      <c r="N2" s="14">
         <f>P_plus*f^2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O2" s="14" t="e">
+        <v>0</v>
+      </c>
+      <c r="O2" s="14">
         <f>P_plus*f^3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P2" s="14" t="e">
+        <v>0</v>
+      </c>
+      <c r="P2" s="14">
         <f>P_plus*f^4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q2" s="14" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14">
         <f>P_plus*f^5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R2" s="14" t="e">
+        <v>0</v>
+      </c>
+      <c r="R2" s="14">
         <f>(M_plus + P_plus)*f</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S2" s="14" t="e">
+        <v>1.2249999999999999E-7</v>
+      </c>
+      <c r="S2" s="14">
         <f>(M_plus + P_plus)*f^2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T2" s="14" t="e">
+        <v>4.2874999999999994E-11</v>
+      </c>
+      <c r="T2" s="14">
         <f>(M_plus + P_plus)*f^3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U2" s="14" t="e">
+        <v>1.5006249999999997E-14</v>
+      </c>
+      <c r="U2" s="14">
         <f>(M_plus + P_plus)*f^4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V2" s="14" t="e">
+        <v>5.2521874999999988E-18</v>
+      </c>
+      <c r="V2" s="14">
         <f>(M_plus + P_plus)*f^5</f>
-        <v>#VALUE!</v>
+        <v>1.8382656249999994E-21</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
@@ -2516,17 +1942,17 @@
       <c r="C3" s="7">
         <v>0</v>
       </c>
-      <c r="D3" s="14" t="str">
+      <c r="D3" s="14">
         <f>k_unmature</f>
-        <v>k_unmature</v>
-      </c>
-      <c r="E3" s="14" t="str">
+        <v>0.378</v>
+      </c>
+      <c r="E3" s="14">
         <f>k_unprime</f>
-        <v>k_unprime</v>
-      </c>
-      <c r="F3" s="14" t="str">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F3" s="14">
         <f>k_refill</f>
-        <v>k_refill</v>
+        <v>0</v>
       </c>
       <c r="G3" s="11">
         <v>0</v>
@@ -2584,9 +2010,9 @@
       <c r="B4" s="11">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="str">
-        <f>k_mature</f>
-        <v>k_mature</v>
+      <c r="C4" s="15">
+        <f>k_mature_basal</f>
+        <v>0</v>
       </c>
       <c r="D4" s="13">
         <v>0</v>
@@ -2597,13 +2023,13 @@
       <c r="F4" s="11">
         <v>0</v>
       </c>
-      <c r="G4" s="14" t="str">
+      <c r="G4" s="14">
         <f>k_unprime</f>
-        <v>k_unprime</v>
-      </c>
-      <c r="H4" s="14" t="str">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H4" s="14">
         <f>k_off</f>
-        <v>k_off</v>
+        <v>4</v>
       </c>
       <c r="I4" s="11">
         <v>0</v>
@@ -2655,9 +2081,8 @@
       <c r="B5" s="11">
         <v>0</v>
       </c>
-      <c r="C5" s="12" t="str">
-        <f>k_prime</f>
-        <v>k_prime</v>
+      <c r="C5" s="15">
+        <v>0</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
@@ -2668,9 +2093,9 @@
       <c r="F5" s="11">
         <v>0</v>
       </c>
-      <c r="G5" s="14" t="str">
+      <c r="G5" s="14">
         <f>k_unmature</f>
-        <v>k_unmature</v>
+        <v>0.378</v>
       </c>
       <c r="H5" s="11">
         <v>0</v>
@@ -2687,9 +2112,9 @@
       <c r="L5" s="11">
         <v>0</v>
       </c>
-      <c r="M5" s="14" t="str">
+      <c r="M5" s="14">
         <f>k_off</f>
-        <v>k_off</v>
+        <v>4</v>
       </c>
       <c r="N5" s="11">
         <v>0</v>
@@ -2797,18 +2222,16 @@
       <c r="C7" s="11">
         <v>0</v>
       </c>
-      <c r="D7" s="12" t="str">
-        <f>k_prime</f>
-        <v>k_prime</v>
-      </c>
-      <c r="E7" s="12" t="str">
-        <f>k_mature</f>
-        <v>k_mature</v>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
       </c>
       <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="16">
         <v>0</v>
       </c>
       <c r="H7" s="11">
@@ -2841,9 +2264,9 @@
       <c r="Q7" s="11">
         <v>0</v>
       </c>
-      <c r="R7" s="14" t="str">
+      <c r="R7" s="14">
         <f>k_off</f>
-        <v>k_off</v>
+        <v>4</v>
       </c>
       <c r="S7" s="11">
         <v>0</v>
@@ -2868,9 +2291,8 @@
       <c r="C8" s="11">
         <v>0</v>
       </c>
-      <c r="D8" s="12" t="e">
-        <f>5*k_on</f>
-        <v>#VALUE!</v>
+      <c r="D8" s="11">
+        <v>0</v>
       </c>
       <c r="E8" s="11">
         <v>0</v>
@@ -2881,12 +2303,12 @@
       <c r="G8" s="11">
         <v>0</v>
       </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="14" t="e">
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
         <f>2*b*k_off</f>
-        <v>#VALUE!</v>
+        <v>4</v>
       </c>
       <c r="J8" s="11">
         <v>0</v>
@@ -2950,16 +2372,15 @@
       <c r="G9" s="11">
         <v>0</v>
       </c>
-      <c r="H9" s="12" t="e">
-        <f>4*k_on</f>
-        <v>#VALUE!</v>
+      <c r="H9" s="11">
+        <v>0</v>
       </c>
       <c r="I9" s="7">
         <v>0</v>
       </c>
-      <c r="J9" s="14" t="e">
+      <c r="J9" s="14">
         <f>3*b^2*k_off</f>
-        <v>#VALUE!</v>
+        <v>3</v>
       </c>
       <c r="K9" s="11">
         <v>0</v>
@@ -3023,16 +2444,15 @@
       <c r="H10" s="11">
         <v>0</v>
       </c>
-      <c r="I10" s="12" t="e">
-        <f>3*k_on</f>
-        <v>#VALUE!</v>
+      <c r="I10" s="11">
+        <v>0</v>
       </c>
       <c r="J10" s="7">
         <v>0</v>
       </c>
-      <c r="K10" s="14" t="e">
+      <c r="K10" s="14">
         <f>4*b^3*k_off</f>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
       <c r="L10" s="11">
         <v>0</v>
@@ -3096,16 +2516,15 @@
       <c r="I11" s="11">
         <v>0</v>
       </c>
-      <c r="J11" s="12" t="e">
-        <f>2*k_on</f>
-        <v>#VALUE!</v>
+      <c r="J11" s="11">
+        <v>0</v>
       </c>
       <c r="K11" s="7">
         <v>0</v>
       </c>
-      <c r="L11" s="14" t="e">
+      <c r="L11" s="14">
         <f>5*b^4*k_off</f>
-        <v>#VALUE!</v>
+        <v>1.25</v>
       </c>
       <c r="M11" s="11">
         <v>0</v>
@@ -3169,9 +2588,8 @@
       <c r="J12" s="11">
         <v>0</v>
       </c>
-      <c r="K12" s="12" t="str">
-        <f>k_on</f>
-        <v>k_on</v>
+      <c r="K12" s="11">
+        <v>0</v>
       </c>
       <c r="L12" s="7">
         <v>0</v>
@@ -3220,9 +2638,8 @@
       <c r="D13" s="11">
         <v>0</v>
       </c>
-      <c r="E13" s="12" t="e">
-        <f>5*k_on</f>
-        <v>#VALUE!</v>
+      <c r="E13" s="11">
+        <v>0</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
@@ -3248,9 +2665,9 @@
       <c r="M13" s="7">
         <v>0</v>
       </c>
-      <c r="N13" s="14" t="e">
+      <c r="N13" s="14">
         <f>2*b*k_off</f>
-        <v>#VALUE!</v>
+        <v>4</v>
       </c>
       <c r="O13" s="11">
         <v>0</v>
@@ -3314,16 +2731,15 @@
       <c r="L14" s="11">
         <v>0</v>
       </c>
-      <c r="M14" s="12" t="e">
-        <f>4*k_on</f>
-        <v>#VALUE!</v>
+      <c r="M14" s="11">
+        <v>0</v>
       </c>
       <c r="N14" s="7">
         <v>0</v>
       </c>
-      <c r="O14" s="14" t="e">
+      <c r="O14" s="14">
         <f>3*b^2*k_off</f>
-        <v>#VALUE!</v>
+        <v>3</v>
       </c>
       <c r="P14" s="11">
         <v>0</v>
@@ -3387,16 +2803,15 @@
       <c r="M15" s="11">
         <v>0</v>
       </c>
-      <c r="N15" s="12" t="e">
-        <f>3*k_on</f>
-        <v>#VALUE!</v>
+      <c r="N15" s="11">
+        <v>0</v>
       </c>
       <c r="O15" s="7">
         <v>0</v>
       </c>
-      <c r="P15" s="14" t="e">
+      <c r="P15" s="14">
         <f>4*b^3*k_off</f>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="11">
         <v>0</v>
@@ -3460,16 +2875,15 @@
       <c r="N16" s="11">
         <v>0</v>
       </c>
-      <c r="O16" s="12" t="e">
-        <f>2*k_on</f>
-        <v>#VALUE!</v>
+      <c r="O16" s="11">
+        <v>0</v>
       </c>
       <c r="P16" s="7">
         <v>0</v>
       </c>
-      <c r="Q16" s="14" t="e">
+      <c r="Q16" s="14">
         <f>5*b^4*k_off</f>
-        <v>#VALUE!</v>
+        <v>1.25</v>
       </c>
       <c r="R16" s="11">
         <v>0</v>
@@ -3533,9 +2947,8 @@
       <c r="O17" s="11">
         <v>0</v>
       </c>
-      <c r="P17" s="12" t="str">
-        <f>k_on</f>
-        <v>k_on</v>
+      <c r="P17" s="11">
+        <v>0</v>
       </c>
       <c r="Q17" s="7">
         <v>0</v>
@@ -3575,9 +2988,8 @@
       <c r="F18" s="11">
         <v>0</v>
       </c>
-      <c r="G18" s="12" t="e">
-        <f>5*k_on</f>
-        <v>#VALUE!</v>
+      <c r="G18" s="11">
+        <v>0</v>
       </c>
       <c r="H18" s="11">
         <v>0</v>
@@ -3612,9 +3024,9 @@
       <c r="R18" s="7">
         <v>0</v>
       </c>
-      <c r="S18" s="14" t="e">
+      <c r="S18" s="14">
         <f>2*b*k_off</f>
-        <v>#VALUE!</v>
+        <v>4</v>
       </c>
       <c r="T18" s="11">
         <v>0</v>
@@ -3678,16 +3090,15 @@
       <c r="Q19" s="11">
         <v>0</v>
       </c>
-      <c r="R19" s="12" t="e">
-        <f>4*k_on</f>
-        <v>#VALUE!</v>
+      <c r="R19" s="11">
+        <v>0</v>
       </c>
       <c r="S19" s="7">
         <v>0</v>
       </c>
-      <c r="T19" s="14" t="e">
+      <c r="T19" s="14">
         <f>3*b^2*k_off</f>
-        <v>#VALUE!</v>
+        <v>3</v>
       </c>
       <c r="U19" s="11">
         <v>0</v>
@@ -3751,16 +3162,15 @@
       <c r="R20" s="11">
         <v>0</v>
       </c>
-      <c r="S20" s="12" t="e">
-        <f>3*k_on</f>
-        <v>#VALUE!</v>
+      <c r="S20" s="11">
+        <v>0</v>
       </c>
       <c r="T20" s="7">
         <v>0</v>
       </c>
-      <c r="U20" s="14" t="e">
+      <c r="U20" s="14">
         <f>4*b^3*k_off</f>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
       <c r="V20" s="11">
         <v>0</v>
@@ -3824,16 +3234,15 @@
       <c r="S21" s="11">
         <v>0</v>
       </c>
-      <c r="T21" s="12" t="e">
-        <f>2*k_on</f>
-        <v>#VALUE!</v>
+      <c r="T21" s="11">
+        <v>0</v>
       </c>
       <c r="U21" s="7">
         <v>0</v>
       </c>
-      <c r="V21" s="14" t="e">
+      <c r="V21" s="14">
         <f>5*b^4*k_off</f>
-        <v>#VALUE!</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.25">
@@ -3897,17 +3306,16 @@
       <c r="T22" s="11">
         <v>0</v>
       </c>
-      <c r="U22" s="12" t="str">
-        <f>k_on</f>
-        <v>k_on</v>
+      <c r="U22" s="11">
+        <v>0</v>
       </c>
       <c r="V22" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="24" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>15</v>
@@ -4116,8 +3524,9 @@
       <c r="B27" s="11">
         <v>0</v>
       </c>
-      <c r="C27" s="11">
-        <v>1</v>
+      <c r="C27" s="12">
+        <f>k_mature</f>
+        <v>300000</v>
       </c>
       <c r="D27" s="7">
         <v>0</v>
@@ -4184,8 +3593,9 @@
       <c r="B28" s="11">
         <v>0</v>
       </c>
-      <c r="C28" s="11">
-        <v>1</v>
+      <c r="C28" s="12">
+        <f>k_prime</f>
+        <v>7330</v>
       </c>
       <c r="D28" s="11">
         <v>0</v>
@@ -4323,11 +3733,13 @@
       <c r="C30" s="11">
         <v>0</v>
       </c>
-      <c r="D30" s="11">
-        <v>1</v>
-      </c>
-      <c r="E30" s="11">
-        <v>1</v>
+      <c r="D30" s="12">
+        <f>k_prime</f>
+        <v>7330</v>
+      </c>
+      <c r="E30" s="12">
+        <f>k_mature</f>
+        <v>300000</v>
       </c>
       <c r="F30" s="11">
         <v>0</v>
@@ -4391,8 +3803,9 @@
       <c r="C31" s="11">
         <v>0</v>
       </c>
-      <c r="D31" s="11">
-        <v>1</v>
+      <c r="D31" s="12">
+        <f>5*k_on</f>
+        <v>700000</v>
       </c>
       <c r="E31" s="11">
         <v>0</v>
@@ -4471,8 +3884,9 @@
       <c r="G32" s="11">
         <v>0</v>
       </c>
-      <c r="H32" s="11">
-        <v>1</v>
+      <c r="H32" s="12">
+        <f>4*k_on</f>
+        <v>560000</v>
       </c>
       <c r="I32" s="7">
         <v>0</v>
@@ -4542,8 +3956,9 @@
       <c r="H33" s="11">
         <v>0</v>
       </c>
-      <c r="I33" s="11">
-        <v>1</v>
+      <c r="I33" s="12">
+        <f>3*k_on</f>
+        <v>420000</v>
       </c>
       <c r="J33" s="7">
         <v>0</v>
@@ -4613,8 +4028,9 @@
       <c r="I34" s="11">
         <v>0</v>
       </c>
-      <c r="J34" s="11">
-        <v>1</v>
+      <c r="J34" s="12">
+        <f>2*k_on</f>
+        <v>280000</v>
       </c>
       <c r="K34" s="7">
         <v>0</v>
@@ -4684,8 +4100,9 @@
       <c r="J35" s="11">
         <v>0</v>
       </c>
-      <c r="K35" s="11">
-        <v>1</v>
+      <c r="K35" s="12">
+        <f>k_on</f>
+        <v>140000</v>
       </c>
       <c r="L35" s="7">
         <v>0</v>
@@ -4734,8 +4151,9 @@
       <c r="D36" s="11">
         <v>0</v>
       </c>
-      <c r="E36" s="11">
-        <v>1</v>
+      <c r="E36" s="12">
+        <f>5*k_on</f>
+        <v>700000</v>
       </c>
       <c r="F36" s="11">
         <v>0</v>
@@ -4826,8 +4244,9 @@
       <c r="L37" s="11">
         <v>0</v>
       </c>
-      <c r="M37" s="11">
-        <v>1</v>
+      <c r="M37" s="12">
+        <f>4*k_on</f>
+        <v>560000</v>
       </c>
       <c r="N37" s="7">
         <v>0</v>
@@ -4897,8 +4316,9 @@
       <c r="M38" s="11">
         <v>0</v>
       </c>
-      <c r="N38" s="11">
-        <v>1</v>
+      <c r="N38" s="12">
+        <f>3*k_on</f>
+        <v>420000</v>
       </c>
       <c r="O38" s="7">
         <v>0</v>
@@ -4968,8 +4388,9 @@
       <c r="N39" s="11">
         <v>0</v>
       </c>
-      <c r="O39" s="11">
-        <v>1</v>
+      <c r="O39" s="12">
+        <f>2*k_on</f>
+        <v>280000</v>
       </c>
       <c r="P39" s="7">
         <v>0</v>
@@ -5039,8 +4460,9 @@
       <c r="O40" s="11">
         <v>0</v>
       </c>
-      <c r="P40" s="11">
-        <v>1</v>
+      <c r="P40" s="12">
+        <f>k_on</f>
+        <v>140000</v>
       </c>
       <c r="Q40" s="7">
         <v>0</v>
@@ -5080,8 +4502,9 @@
       <c r="F41" s="11">
         <v>0</v>
       </c>
-      <c r="G41" s="11">
-        <v>1</v>
+      <c r="G41" s="12">
+        <f>5*k_on</f>
+        <v>700000</v>
       </c>
       <c r="H41" s="11">
         <v>0</v>
@@ -5181,8 +4604,9 @@
       <c r="Q42" s="11">
         <v>0</v>
       </c>
-      <c r="R42" s="11">
-        <v>1</v>
+      <c r="R42" s="12">
+        <f>4*k_on</f>
+        <v>560000</v>
       </c>
       <c r="S42" s="7">
         <v>0</v>
@@ -5252,8 +4676,9 @@
       <c r="R43" s="11">
         <v>0</v>
       </c>
-      <c r="S43" s="11">
-        <v>1</v>
+      <c r="S43" s="12">
+        <f>3*k_on</f>
+        <v>420000</v>
       </c>
       <c r="T43" s="7">
         <v>0</v>
@@ -5323,8 +4748,9 @@
       <c r="S44" s="11">
         <v>0</v>
       </c>
-      <c r="T44" s="11">
-        <v>1</v>
+      <c r="T44" s="12">
+        <f>2*k_on</f>
+        <v>280000</v>
       </c>
       <c r="U44" s="7">
         <v>0</v>
@@ -5394,8 +4820,9 @@
       <c r="T45" s="11">
         <v>0</v>
       </c>
-      <c r="U45" s="11">
-        <v>1</v>
+      <c r="U45" s="12">
+        <f>k_on</f>
+        <v>140000</v>
       </c>
       <c r="V45" s="7">
         <v>0</v>
@@ -5403,13 +4830,13 @@
     </row>
     <row r="47" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="C47" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" x14ac:dyDescent="0.25">
@@ -5422,81 +4849,89 @@
     </row>
     <row r="49" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B49" s="6">
+        <v>83</v>
+      </c>
+      <c r="B49" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="6">
         <v>300000</v>
-      </c>
-    </row>
-    <row r="50" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="6">
-        <v>0.378</v>
       </c>
     </row>
     <row r="51" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B51" s="6">
-        <v>7330</v>
+        <v>0.378</v>
       </c>
     </row>
     <row r="52" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B52" s="6">
-        <v>0.010999999999999999</v>
+        <v>7330</v>
       </c>
     </row>
     <row r="53" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B53" s="6">
-        <v>140000</v>
+        <v>0.010999999999999999</v>
       </c>
     </row>
     <row r="54" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B54" s="6">
-        <v>4</v>
+        <v>140000</v>
       </c>
     </row>
     <row r="55" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B55" s="6">
-        <v>0.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B56" s="6">
-        <v>28</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B57" s="6">
-        <v>0.00035</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B58" s="6">
+        <v>0.00035</v>
+      </c>
+    </row>
+    <row r="59" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="6">
         <v>0.00035</v>
       </c>
     </row>

</xml_diff>